<commit_message>
PRM6: norm(similarity) + position
</commit_message>
<xml_diff>
--- a/develop/PRM_comparsion.xlsx
+++ b/develop/PRM_comparsion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melody/Code/NANet/develop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321B53EA-3729-5146-9655-DD9A6DD59A8C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C48620-0CBA-FB42-9E30-25ADAA5B7A2D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14480" xr2:uid="{B3BB4FD7-8D27-024B-A700-38D589DD4097}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
   <si>
     <t>IJCAI2020</t>
   </si>
@@ -115,6 +115,15 @@
   </si>
   <si>
     <t>std+1e-7 not 1e-5 (replace line 5)</t>
+  </si>
+  <si>
+    <t>prm5_resnet50</t>
+  </si>
+  <si>
+    <t>temp4</t>
+  </si>
+  <si>
+    <t>too lower; conv slow</t>
   </si>
 </sst>
 </file>
@@ -512,12 +521,12 @@
   <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="10" max="10" width="17" customWidth="1"/>
+    <col min="10" max="10" width="18.5" customWidth="1"/>
     <col min="11" max="11" width="38.5" customWidth="1"/>
     <col min="12" max="12" width="41.33203125" customWidth="1"/>
   </cols>
@@ -769,23 +778,45 @@
       <c r="I8" s="1">
         <v>64</v>
       </c>
-      <c r="J8" s="1"/>
+      <c r="J8" s="6" t="s">
+        <v>32</v>
+      </c>
       <c r="K8" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="20" customHeight="1">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
+      <c r="A9" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="5">
+        <v>4</v>
+      </c>
+      <c r="C9" s="5">
+        <v>16</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="5">
+        <v>16</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="5">
+        <v>64</v>
+      </c>
       <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
+      <c r="K9" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="10" spans="1:12" ht="20" customHeight="1">
       <c r="A10" s="1"/>

</xml_diff>

<commit_message>
prm9: add e^(-x) to distance
</commit_message>
<xml_diff>
--- a/develop/PRM_comparsion.xlsx
+++ b/develop/PRM_comparsion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melody/Code/NANet/develop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F032D13E-5500-A744-8FAB-C65AEE887B7E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C218D9D2-F0CC-C94E-85F6-4D00F2489C2C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14480" xr2:uid="{B3BB4FD7-8D27-024B-A700-38D589DD4097}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="44">
   <si>
     <t>IJCAI2020</t>
   </si>
@@ -154,13 +154,16 @@
   </si>
   <si>
     <t>remove position</t>
+  </si>
+  <si>
+    <t>prm_8x8_l1norm_resnet50</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -179,6 +182,13 @@
       <sz val="12"/>
       <color theme="4" tint="-0.249977111117893"/>
       <name val="Calibri (Body)_x0000_"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -234,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -247,6 +257,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -564,7 +575,7 @@
   <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -973,7 +984,9 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="20" customHeight="1">
-      <c r="A13" s="1"/>
+      <c r="A13" s="12" t="s">
+        <v>40</v>
+      </c>
       <c r="B13" s="9">
         <v>16</v>
       </c>
@@ -993,7 +1006,7 @@
         <v>32</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="I13" s="10">
         <v>48</v>
@@ -1007,17 +1020,37 @@
       </c>
     </row>
     <row r="14" spans="1:12" ht="20" customHeight="1">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
+      <c r="A14" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="9">
+        <v>8</v>
+      </c>
+      <c r="C14" s="9">
+        <v>8</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="9">
+        <v>32</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="10">
+        <v>48</v>
+      </c>
+      <c r="J14" s="9"/>
+      <c r="K14" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="15" spans="1:12" ht="20" customHeight="1">
       <c r="A15" s="1"/>

</xml_diff>

<commit_message>
PRM10S: looks like PRM10 can achieve the best performance
</commit_message>
<xml_diff>
--- a/develop/PRM_comparsion.xlsx
+++ b/develop/PRM_comparsion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melody/Code/NANet/develop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4994456D-1E3B-544C-8F0E-6277C3DACE56}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6170E2C-A09C-D249-8432-637E0A9F6973}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14480" xr2:uid="{B3BB4FD7-8D27-024B-A700-38D589DD4097}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="56">
   <si>
     <t>IJCAI2020</t>
   </si>
@@ -178,6 +178,21 @@
   </si>
   <si>
     <t>60/15</t>
+  </si>
+  <si>
+    <t>prm11_resnet50</t>
+  </si>
+  <si>
+    <t>prm12_resnet50</t>
+  </si>
+  <si>
+    <t>x+Conv[sig(similarity)*key]</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>se_resnet50</t>
   </si>
 </sst>
 </file>
@@ -272,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -287,6 +302,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -604,7 +622,7 @@
   <dimension ref="A1:M40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1008,9 +1026,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" ht="20" customHeight="1">
-      <c r="A12" s="11" t="s">
-        <v>40</v>
-      </c>
+      <c r="A12" s="11"/>
       <c r="B12" s="1" t="s">
         <v>48</v>
       </c>
@@ -1049,9 +1065,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" ht="20" customHeight="1">
-      <c r="A13" s="12" t="s">
-        <v>40</v>
-      </c>
+      <c r="A13" s="12"/>
       <c r="B13" s="1" t="s">
         <v>48</v>
       </c>
@@ -1090,9 +1104,7 @@
       </c>
     </row>
     <row r="14" spans="1:13" ht="20" customHeight="1">
-      <c r="A14" s="12" t="s">
-        <v>40</v>
-      </c>
+      <c r="A14" s="12"/>
       <c r="B14" s="1" t="s">
         <v>48</v>
       </c>
@@ -1128,9 +1140,7 @@
       </c>
     </row>
     <row r="15" spans="1:13" ht="20" customHeight="1">
-      <c r="A15" s="12" t="s">
-        <v>40</v>
-      </c>
+      <c r="A15" s="12"/>
       <c r="B15" s="1" t="s">
         <v>48</v>
       </c>
@@ -1169,7 +1179,9 @@
       </c>
     </row>
     <row r="16" spans="1:13" ht="20" customHeight="1">
-      <c r="A16" s="12"/>
+      <c r="A16" s="12" t="s">
+        <v>40</v>
+      </c>
       <c r="B16" s="13" t="s">
         <v>50</v>
       </c>
@@ -1189,11 +1201,13 @@
         <v>10</v>
       </c>
       <c r="H16" s="5">
-        <v>16</v>
-      </c>
-      <c r="I16" s="1"/>
+        <v>32</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="J16" s="5">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="K16" s="1"/>
       <c r="L16" s="5" t="s">
@@ -1203,49 +1217,113 @@
         <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="20" customHeight="1">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-    </row>
-    <row r="18" spans="1:12" ht="20" customHeight="1">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-    </row>
-    <row r="19" spans="1:12" ht="20" customHeight="1">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
+    <row r="17" spans="1:13" ht="20" customHeight="1">
+      <c r="A17" s="12"/>
+      <c r="B17" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="5">
+        <v>16</v>
+      </c>
+      <c r="D17" s="5">
+        <v>4</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="5">
+        <v>16</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J17" s="5">
+        <v>64</v>
+      </c>
+      <c r="K17" s="5">
+        <v>74.13</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="M17" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="20" customHeight="1">
+      <c r="A18" s="12"/>
+      <c r="B18" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="5">
+        <v>4</v>
+      </c>
+      <c r="D18" s="5">
+        <v>32</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="5">
+        <v>16</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J18" s="5">
+        <v>64</v>
+      </c>
+      <c r="K18" s="5">
+        <v>73.989999999999995</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="M18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="20" customHeight="1">
+      <c r="A19" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="5">
+        <v>16</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J19" s="5">
+        <v>64</v>
+      </c>
       <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-    </row>
-    <row r="20" spans="1:12" ht="20" customHeight="1">
+      <c r="L19" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="20" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1259,7 +1337,7 @@
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="1:12" ht="20" customHeight="1">
+    <row r="21" spans="1:13" ht="20" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1273,7 +1351,7 @@
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:12" ht="20" customHeight="1">
+    <row r="22" spans="1:13" ht="20" customHeight="1">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1287,7 +1365,7 @@
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:12" ht="20" customHeight="1">
+    <row r="23" spans="1:13" ht="20" customHeight="1">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1301,17 +1379,17 @@
       <c r="K23" s="3"/>
       <c r="L23" s="3"/>
     </row>
-    <row r="24" spans="1:12" ht="20" customHeight="1"/>
-    <row r="25" spans="1:12" ht="20" customHeight="1">
+    <row r="24" spans="1:13" ht="20" customHeight="1"/>
+    <row r="25" spans="1:13" ht="20" customHeight="1">
       <c r="L25" s="4"/>
     </row>
-    <row r="26" spans="1:12" ht="20" customHeight="1"/>
-    <row r="27" spans="1:12" ht="20" customHeight="1"/>
-    <row r="28" spans="1:12" ht="20" customHeight="1"/>
-    <row r="29" spans="1:12" ht="20" customHeight="1"/>
-    <row r="30" spans="1:12" ht="20" customHeight="1"/>
-    <row r="31" spans="1:12" ht="20" customHeight="1"/>
-    <row r="32" spans="1:12" ht="20" customHeight="1"/>
+    <row r="26" spans="1:13" ht="20" customHeight="1"/>
+    <row r="27" spans="1:13" ht="20" customHeight="1"/>
+    <row r="28" spans="1:13" ht="20" customHeight="1"/>
+    <row r="29" spans="1:13" ht="20" customHeight="1"/>
+    <row r="30" spans="1:13" ht="20" customHeight="1"/>
+    <row r="31" spans="1:13" ht="20" customHeight="1"/>
+    <row r="32" spans="1:13" ht="20" customHeight="1"/>
     <row r="33" ht="20" customHeight="1"/>
     <row r="34" ht="20" customHeight="1"/>
     <row r="35" ht="20" customHeight="1"/>
@@ -1321,6 +1399,9 @@
     <row r="39" ht="20" customHeight="1"/>
     <row r="40" ht="20" customHeight="1"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C19:G19"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
prm15_2: dotproduct/sqrt(each group channels) (mean+max)/2
</commit_message>
<xml_diff>
--- a/develop/PRM_comparsion.xlsx
+++ b/develop/PRM_comparsion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melody/Code/NANet/develop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{965836B5-2B9B-5240-837A-91B8F32E9876}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40FE1AA-EAAD-C948-B3DE-4A5CE14C30EE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14480" xr2:uid="{B3BB4FD7-8D27-024B-A700-38D589DD4097}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="68">
   <si>
     <t>IJCAI2020</t>
   </si>
@@ -220,6 +220,15 @@
   </si>
   <si>
     <t>sge_resnet50</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>prm15_resnet50</t>
+  </si>
+  <si>
+    <t>based on SGE, add max_value to GAP</t>
   </si>
 </sst>
 </file>
@@ -647,8 +656,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A868B19E-AFD6-AC47-B1AB-8C6DFD803BD5}">
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1407,7 +1416,7 @@
       <c r="A22" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="11" t="s">
         <v>50</v>
       </c>
       <c r="C22" s="3">
@@ -1520,7 +1529,7 @@
       </c>
     </row>
     <row r="25" spans="1:13" ht="20" customHeight="1">
-      <c r="B25" s="11" t="s">
+      <c r="B25" s="1" t="s">
         <v>48</v>
       </c>
       <c r="C25" s="17" t="s">
@@ -1543,7 +1552,41 @@
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="20" customHeight="1"/>
+    <row r="26" spans="1:13" ht="20" customHeight="1">
+      <c r="B26" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" s="3">
+        <v>64</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H26" s="3">
+        <v>32</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J26" s="3">
+        <v>32</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="M26" t="s">
+        <v>67</v>
+      </c>
+    </row>
     <row r="27" spans="1:13" ht="20" customHeight="1"/>
     <row r="28" spans="1:13" ht="20" customHeight="1"/>
     <row r="29" spans="1:13" ht="20" customHeight="1"/>

</xml_diff>

<commit_message>
PRM16: add a embedding to prm15_2
</commit_message>
<xml_diff>
--- a/develop/PRM_comparsion.xlsx
+++ b/develop/PRM_comparsion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melody/Code/NANet/develop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{148404F6-DE74-CF43-882D-3E9584B2B39C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC4B06D-BD35-A341-B65B-2AFDBFA2A9B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14480" xr2:uid="{B3BB4FD7-8D27-024B-A700-38D589DD4097}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="71">
   <si>
     <t>IJCAI2020</t>
   </si>
@@ -232,6 +232,12 @@
   </si>
   <si>
     <t>not good as sge</t>
+  </si>
+  <si>
+    <t>based on SGE, (mean+max)/2, dotproduct/sqrt(c/g)</t>
+  </si>
+  <si>
+    <t>prm15_2_resnet50</t>
   </si>
 </sst>
 </file>
@@ -659,8 +665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A868B19E-AFD6-AC47-B1AB-8C6DFD803BD5}">
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1493,9 +1499,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" ht="20" customHeight="1">
-      <c r="A24" s="10" t="s">
-        <v>40</v>
-      </c>
+      <c r="A24" s="10"/>
       <c r="B24" s="11" t="s">
         <v>50</v>
       </c>
@@ -1593,7 +1597,45 @@
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="20" customHeight="1"/>
+    <row r="27" spans="1:13" ht="20" customHeight="1">
+      <c r="A27" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" s="3">
+        <v>64</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H27" s="3">
+        <v>16</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J27" s="3">
+        <v>64</v>
+      </c>
+      <c r="K27" s="4"/>
+      <c r="L27" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="M27" t="s">
+        <v>69</v>
+      </c>
+    </row>
     <row r="28" spans="1:13" ht="20" customHeight="1"/>
     <row r="29" spans="1:13" ht="20" customHeight="1"/>
     <row r="30" spans="1:13" ht="20" customHeight="1"/>

</xml_diff>